<commit_message>
lesson 3 & 4 updates
</commit_message>
<xml_diff>
--- a/Lesson3/hometask/module_script/clients_wbp_prices/monty/Monty_mwp_price_07072022.xlsx
+++ b/Lesson3/hometask/module_script/clients_wbp_prices/monty/Monty_mwp_price_07072022.xlsx
@@ -108,10 +108,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>608914</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>37643</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>303086</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>113500</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -129,7 +129,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1219200" y="190500"/>
-          <a:ext cx="5485714" cy="3657143"/>
+          <a:ext cx="13714286" cy="6400000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -735,7 +735,7 @@
         <v>44773</v>
       </c>
       <c r="B39">
-        <v>1901.1</v>
+        <v>1906.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>